<commit_message>
added rules for Stopping area and Workzones
added rules for Stopping area and Workzones
</commit_message>
<xml_diff>
--- a/DTVT_BLUE/Results/Test_Results_NOK_RULE_TMS_PLATF_0003.xlsx
+++ b/DTVT_BLUE/Results/Test_Results_NOK_RULE_TMS_PLATF_0003.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Test_Results" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test_Results" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>